<commit_message>
Module & gaand faad questions
</commit_message>
<xml_diff>
--- a/GreateProblemsCollections.xlsx
+++ b/GreateProblemsCollections.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t xml:space="preserve">Sl No.</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t xml:space="preserve">frq from 1 to 51 and do – when needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codeforces.com/contest/1285/problem/C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LCM property use hoga</t>
   </si>
 </sst>
 </file>
@@ -374,10 +380,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -476,6 +482,14 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
800 rated cp sheet
</commit_message>
<xml_diff>
--- a/GreateProblemsCollections.xlsx
+++ b/GreateProblemsCollections.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t xml:space="preserve">Sl No.</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t xml:space="preserve">LCM property use hoga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codeforces.com/problemset/problem/1881/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how tpo find subset of a strig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temp.found(s) != string::npos (use to checl if s is a subset of temp or not and string::npose means tring not found</t>
   </si>
 </sst>
 </file>
@@ -86,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -122,6 +131,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -172,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,6 +209,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -380,10 +398,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,6 +508,17 @@
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gaand faad solved and complete module 10
</commit_message>
<xml_diff>
--- a/GreateProblemsCollections.xlsx
+++ b/GreateProblemsCollections.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t xml:space="preserve">Sl No.</t>
   </si>
@@ -86,6 +86,33 @@
   </si>
   <si>
     <t xml:space="preserve">temp.found(s) != string::npos (use to checl if s is a subset of temp or not and string::npose means tring not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codeforces.com/problemset/problem/1904/B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dinamic Programming lagega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://cses.fi/problemset/task/1643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kadanes algorithm use hoga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codeforces.com/problemset/problem/1899/C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codeforces.com/problemset/problem/1873/E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Search problem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://codeforces.com/problemset/problem/1827/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary Search problem upperbound related</t>
   </si>
 </sst>
 </file>
@@ -95,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -132,11 +159,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -186,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -211,7 +233,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,10 +424,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,6 +521,9 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -503,6 +532,9 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -511,6 +543,9 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
@@ -521,7 +556,63 @@
         <v>21</v>
       </c>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C11:C12"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://leetcode.com/problems/sudoku-solver/"/>
     <hyperlink ref="B3" r:id="rId2" display="https://leetcode.com/problems/n-queens/"/>

</xml_diff>